<commit_message>
Add Admins Category working list working createCategory working editCategory working deleteCategory
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programing\AngularJS\AngularJSApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="61">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -170,9 +170,6 @@
     <t>GitHub (up to 100)</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Basic Options (up to 130)</t>
   </si>
   <si>
@@ -198,13 +195,25 @@
   </si>
   <si>
     <t>∞</t>
+  </si>
+  <si>
+    <t>crazy7</t>
+  </si>
+  <si>
+    <t>Veselin Ivelinov Penev</t>
+  </si>
+  <si>
+    <t>https://github.com/veselinpenev/AngularJSApp</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,6 +243,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -329,10 +346,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -360,6 +378,18 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -372,20 +402,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -666,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,7 +701,7 @@
   <sheetData>
     <row r="2" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>46</v>
@@ -688,48 +710,54 @@
         <v>25</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
+      <c r="B3" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
+        <v>51</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
+        <v>53</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
     </row>
     <row r="6" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
+        <v>50</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
@@ -737,7 +765,7 @@
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E8" s="6"/>
     </row>
@@ -747,24 +775,24 @@
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B10" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
+      <c r="B10" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>48</v>
+      <c r="C11" s="5">
+        <v>9</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>3</v>
@@ -775,7 +803,9 @@
       <c r="B12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="5">
+        <v>5</v>
+      </c>
       <c r="D12" s="5" t="s">
         <v>5</v>
       </c>
@@ -785,7 +815,9 @@
       <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="5">
+        <v>5</v>
+      </c>
       <c r="D13" s="5" t="s">
         <v>5</v>
       </c>
@@ -805,7 +837,9 @@
       <c r="B15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="5"/>
+      <c r="C15" s="5">
+        <v>5</v>
+      </c>
       <c r="D15" s="5" t="s">
         <v>5</v>
       </c>
@@ -815,7 +849,9 @@
       <c r="B16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="5"/>
+      <c r="C16" s="5">
+        <v>5</v>
+      </c>
       <c r="D16" s="5" t="s">
         <v>5</v>
       </c>
@@ -825,7 +861,9 @@
       <c r="B17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="5"/>
+      <c r="C17" s="5">
+        <v>10</v>
+      </c>
       <c r="D17" s="5" t="s">
         <v>3</v>
       </c>
@@ -835,7 +873,9 @@
       <c r="B18" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="5"/>
+      <c r="C18" s="5">
+        <v>5</v>
+      </c>
       <c r="D18" s="5" t="s">
         <v>5</v>
       </c>
@@ -845,7 +885,9 @@
       <c r="B19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="5"/>
+      <c r="C19" s="5">
+        <v>10</v>
+      </c>
       <c r="D19" s="5" t="s">
         <v>3</v>
       </c>
@@ -855,7 +897,9 @@
       <c r="B20" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="5"/>
+      <c r="C20" s="5">
+        <v>5</v>
+      </c>
       <c r="D20" s="5" t="s">
         <v>5</v>
       </c>
@@ -865,7 +909,9 @@
       <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="5"/>
+      <c r="C21" s="5">
+        <v>5</v>
+      </c>
       <c r="D21" s="5" t="s">
         <v>5</v>
       </c>
@@ -875,7 +921,9 @@
       <c r="B22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="5"/>
+      <c r="C22" s="5">
+        <v>5</v>
+      </c>
       <c r="D22" s="5" t="s">
         <v>5</v>
       </c>
@@ -895,7 +943,9 @@
       <c r="B24" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="5"/>
+      <c r="C24" s="5">
+        <v>5</v>
+      </c>
       <c r="D24" s="5" t="s">
         <v>5</v>
       </c>
@@ -905,7 +955,9 @@
       <c r="B25" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="5"/>
+      <c r="C25" s="5">
+        <v>5</v>
+      </c>
       <c r="D25" s="5" t="s">
         <v>5</v>
       </c>
@@ -915,7 +967,9 @@
       <c r="B26" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="5"/>
+      <c r="C26" s="5">
+        <v>10</v>
+      </c>
       <c r="D26" s="5" t="s">
         <v>3</v>
       </c>
@@ -925,7 +979,9 @@
       <c r="B27" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="5"/>
+      <c r="C27" s="5">
+        <v>5</v>
+      </c>
       <c r="D27" s="5" t="s">
         <v>5</v>
       </c>
@@ -935,7 +991,9 @@
       <c r="B28" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="5"/>
+      <c r="C28" s="5">
+        <v>5</v>
+      </c>
       <c r="D28" s="5" t="s">
         <v>5</v>
       </c>
@@ -945,7 +1003,9 @@
       <c r="B29" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="5"/>
+      <c r="C29" s="5">
+        <v>5</v>
+      </c>
       <c r="D29" s="5" t="s">
         <v>5</v>
       </c>
@@ -955,7 +1015,9 @@
       <c r="B30" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="5"/>
+      <c r="C30" s="5">
+        <v>5</v>
+      </c>
       <c r="D30" s="5" t="s">
         <v>5</v>
       </c>
@@ -965,7 +1027,9 @@
       <c r="B31" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C31" s="5"/>
+      <c r="C31" s="5">
+        <v>5</v>
+      </c>
       <c r="D31" s="5" t="s">
         <v>5</v>
       </c>
@@ -975,25 +1039,29 @@
       <c r="B32" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="5"/>
+      <c r="C32" s="5">
+        <v>5</v>
+      </c>
       <c r="D32" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E32" s="5"/>
     </row>
     <row r="33" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B33" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="20"/>
+      <c r="B33" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="16"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="7"/>
+      <c r="C34" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D34" s="7" t="s">
         <v>28</v>
       </c>
@@ -1003,7 +1071,9 @@
       <c r="B35" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="7"/>
+      <c r="C35" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D35" s="7" t="s">
         <v>28</v>
       </c>
@@ -1013,7 +1083,9 @@
       <c r="B36" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C36" s="7"/>
+      <c r="C36" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D36" s="7" t="s">
         <v>28</v>
       </c>
@@ -1023,7 +1095,9 @@
       <c r="B37" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="7"/>
+      <c r="C37" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D37" s="7" t="s">
         <v>28</v>
       </c>
@@ -1033,7 +1107,9 @@
       <c r="B38" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C38" s="7"/>
+      <c r="C38" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D38" s="7" t="s">
         <v>28</v>
       </c>
@@ -1083,7 +1159,9 @@
       <c r="B43" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C43" s="7"/>
+      <c r="C43" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D43" s="7" t="s">
         <v>28</v>
       </c>
@@ -1093,7 +1171,9 @@
       <c r="B44" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C44" s="7"/>
+      <c r="C44" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D44" s="7" t="s">
         <v>28</v>
       </c>
@@ -1103,7 +1183,9 @@
       <c r="B45" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C45" s="7"/>
+      <c r="C45" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D45" s="7" t="s">
         <v>28</v>
       </c>
@@ -1113,7 +1195,9 @@
       <c r="B46" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C46" s="7"/>
+      <c r="C46" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D46" s="7" t="s">
         <v>28</v>
       </c>
@@ -1165,7 +1249,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>0</v>
+        <v>119</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>
@@ -1182,7 +1266,10 @@
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="C7:E7"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C7" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add admins user menu, and paging
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="JS-SPA-Self-Evaluation-Protocol" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="61">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -399,10 +399,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -689,7 +689,7 @@
   <dimension ref="B2:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:E10"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,11 +753,11 @@
       <c r="B7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
@@ -827,7 +827,9 @@
       <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="D14" s="5" t="s">
         <v>5</v>
       </c>
@@ -933,7 +935,9 @@
       <c r="B23" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="5"/>
+      <c r="C23" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="D23" s="5" t="s">
         <v>5</v>
       </c>
@@ -1119,7 +1123,9 @@
       <c r="B39" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C39" s="7"/>
+      <c r="C39" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D39" s="7" t="s">
         <v>28</v>
       </c>
@@ -1129,7 +1135,9 @@
       <c r="B40" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="7"/>
+      <c r="C40" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D40" s="7" t="s">
         <v>28</v>
       </c>
@@ -1139,7 +1147,9 @@
       <c r="B41" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="7"/>
+      <c r="C41" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D41" s="7" t="s">
         <v>28</v>
       </c>
@@ -1149,7 +1159,9 @@
       <c r="B42" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C42" s="7"/>
+      <c r="C42" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D42" s="7" t="s">
         <v>28</v>
       </c>

</xml_diff>